<commit_message>
Se mejoro el codigo para reducir codigo y hacerlo escalable
</commit_message>
<xml_diff>
--- a/Lista_de_Sensores_HGAS.xlsx
+++ b/Lista_de_Sensores_HGAS.xlsx
@@ -106,7 +106,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -118,6 +118,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -141,6 +142,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -149,13 +157,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -175,6 +176,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -183,13 +191,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -558,39 +559,39 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" style="5" min="1" max="1"/>
-    <col width="11.28515625" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="13.7109375" customWidth="1" style="5" min="3" max="3"/>
-    <col width="39.42578125" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
-    <col width="24.85546875" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col width="14.85546875" customWidth="1" style="5" min="6" max="6"/>
-    <col width="13.140625" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
-    <col width="13.140625" customWidth="1" style="5" min="8" max="8"/>
-    <col width="11.85546875" customWidth="1" style="5" min="9" max="9"/>
-    <col width="13.140625" customWidth="1" style="5" min="10" max="10"/>
-    <col width="14.5703125" customWidth="1" style="5" min="11" max="11"/>
-    <col width="21" customWidth="1" style="5" min="12" max="12"/>
-    <col width="13" customWidth="1" style="5" min="13" max="13"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="5" min="14" max="14"/>
-    <col width="9.7109375" bestFit="1" customWidth="1" style="5" min="15" max="15"/>
+    <col width="10" customWidth="1" style="7" min="1" max="1"/>
+    <col width="11.28515625" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
+    <col width="13.7109375" customWidth="1" style="7" min="3" max="3"/>
+    <col width="39.42578125" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
+    <col width="24.85546875" bestFit="1" customWidth="1" style="7" min="5" max="5"/>
+    <col width="14.85546875" customWidth="1" style="7" min="6" max="6"/>
+    <col width="13.140625" bestFit="1" customWidth="1" style="7" min="7" max="7"/>
+    <col width="13.140625" customWidth="1" style="7" min="8" max="8"/>
+    <col width="11.85546875" customWidth="1" style="7" min="9" max="9"/>
+    <col width="13.140625" customWidth="1" style="7" min="10" max="10"/>
+    <col width="14.5703125" customWidth="1" style="7" min="11" max="11"/>
+    <col width="21" customWidth="1" style="7" min="12" max="12"/>
+    <col width="13" customWidth="1" style="7" min="13" max="13"/>
+    <col width="25.5703125" bestFit="1" customWidth="1" style="7" min="14" max="14"/>
+    <col width="9.7109375" bestFit="1" customWidth="1" style="7" min="15" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.25" customHeight="1" s="5">
+    <row r="1" ht="23.25" customHeight="1" s="7">
       <c r="A1" s="6" t="inlineStr">
         <is>
           <t>RELACION DE SENSORES LEL (VIGENCIA 2 AÑOS)</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="39.75" customHeight="1" s="5">
+    <row r="2" ht="39.75" customHeight="1" s="7">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Barcode</t>
@@ -665,7 +666,7 @@
       </c>
       <c r="O2" s="1" t="n"/>
     </row>
-    <row r="3" ht="24.95" customHeight="1" s="5">
+    <row r="3" ht="24.95" customHeight="1" s="7">
       <c r="A3" t="n">
         <v>1302760</v>
       </c>
@@ -703,7 +704,7 @@
         <v>43686</v>
       </c>
       <c r="I3" t="n">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="J3">
         <f>IF(DAYS360(H3,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -712,8 +713,11 @@
       <c r="L3" s="3" t="n">
         <v>44088.71041666667</v>
       </c>
-    </row>
-    <row r="4" ht="24.95" customHeight="1" s="5">
+      <c r="R3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" ht="24.95" customHeight="1" s="7">
       <c r="A4" t="n">
         <v>1298037</v>
       </c>
@@ -751,7 +755,7 @@
         <v>43476</v>
       </c>
       <c r="I4" t="n">
-        <v>25</v>
+        <v>-5</v>
       </c>
       <c r="J4">
         <f>IF(DAYS360(H4,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -760,8 +764,11 @@
       <c r="L4" s="3" t="n">
         <v>44088.71041666667</v>
       </c>
-    </row>
-    <row r="5" ht="24.95" customHeight="1" s="5">
+      <c r="R4" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" ht="24.95" customHeight="1" s="7">
       <c r="A5" t="n">
         <v>1329257</v>
       </c>
@@ -799,7 +806,7 @@
         <v>43637</v>
       </c>
       <c r="I5" t="n">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="J5">
         <f>IF(DAYS360(H5,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -808,8 +815,11 @@
       <c r="L5" s="3" t="n">
         <v>44088.70972222222</v>
       </c>
-    </row>
-    <row r="6" ht="24.95" customHeight="1" s="5">
+      <c r="R5" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" ht="24.95" customHeight="1" s="7">
       <c r="A6" t="n">
         <v>1302699</v>
       </c>
@@ -847,7 +857,7 @@
         <v>43529</v>
       </c>
       <c r="I6" t="n">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="J6">
         <f>IF(DAYS360(H6,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -857,7 +867,7 @@
         <v>44088.70972222222</v>
       </c>
     </row>
-    <row r="7" ht="24.95" customHeight="1" s="5">
+    <row r="7" ht="24.95" customHeight="1" s="7">
       <c r="A7" t="n">
         <v>1329256</v>
       </c>
@@ -895,7 +905,7 @@
         <v>43871</v>
       </c>
       <c r="I7" t="n">
-        <v>420</v>
+        <v>390</v>
       </c>
       <c r="J7">
         <f>IF(DAYS360(H7,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -910,7 +920,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="24.95" customHeight="1" s="5">
+    <row r="8" ht="24.95" customHeight="1" s="7">
       <c r="A8" t="n">
         <v>1331468</v>
       </c>
@@ -948,7 +958,7 @@
         <v>43500</v>
       </c>
       <c r="I8" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="J8">
         <f>IF(DAYS360(H8,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -958,7 +968,7 @@
         <v>44088.70972222222</v>
       </c>
     </row>
-    <row r="9" ht="24.95" customHeight="1" s="5">
+    <row r="9" ht="24.95" customHeight="1" s="7">
       <c r="A9" t="n">
         <v>1330017</v>
       </c>
@@ -996,7 +1006,7 @@
         <v>43529</v>
       </c>
       <c r="I9" t="n">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="J9">
         <f>IF(DAYS360(H9,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -1006,7 +1016,7 @@
         <v>44088.70902777778</v>
       </c>
     </row>
-    <row r="10" ht="24.95" customHeight="1" s="5">
+    <row r="10" ht="24.95" customHeight="1" s="7">
       <c r="A10" t="n">
         <v>1302765</v>
       </c>
@@ -1044,7 +1054,7 @@
         <v>43666</v>
       </c>
       <c r="I10" t="n">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="J10">
         <f>IF(DAYS360(H10,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -1054,7 +1064,7 @@
         <v>44088.70902777778</v>
       </c>
     </row>
-    <row r="11" ht="24.95" customHeight="1" s="5">
+    <row r="11" ht="24.95" customHeight="1" s="7">
       <c r="A11" t="n">
         <v>1325924</v>
       </c>
@@ -1092,7 +1102,7 @@
         <v>43637</v>
       </c>
       <c r="I11" t="n">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="J11">
         <f>IF(DAYS360(H11,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -1107,7 +1117,7 @@
         <v>44000.56319444445</v>
       </c>
     </row>
-    <row r="12" ht="24.95" customHeight="1" s="5">
+    <row r="12" ht="24.95" customHeight="1" s="7">
       <c r="A12" t="n">
         <v>1398600</v>
       </c>
@@ -1145,7 +1155,7 @@
         <v>43483</v>
       </c>
       <c r="I12" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <f>IF(DAYS360(H12,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -1155,7 +1165,7 @@
         <v>43917.43611111111</v>
       </c>
     </row>
-    <row r="13" ht="24.95" customHeight="1" s="5">
+    <row r="13" ht="24.95" customHeight="1" s="7">
       <c r="A13" t="n">
         <v>1302759</v>
       </c>
@@ -1193,7 +1203,7 @@
         <v>43243</v>
       </c>
       <c r="I13" t="n">
-        <v>-208</v>
+        <v>-238</v>
       </c>
       <c r="J13">
         <f>IF(DAYS360(H13,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -1203,7 +1213,7 @@
         <v>44088.70972222222</v>
       </c>
     </row>
-    <row r="14" ht="24.95" customHeight="1" s="5">
+    <row r="14" ht="24.95" customHeight="1" s="7">
       <c r="A14" t="n">
         <v>1329205</v>
       </c>
@@ -1241,7 +1251,7 @@
         <v>43057</v>
       </c>
       <c r="I14" t="n">
-        <v>-394</v>
+        <v>-424</v>
       </c>
       <c r="J14">
         <f>IF(DAYS360(H14,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -1251,7 +1261,7 @@
         <v>44088.70972222222</v>
       </c>
     </row>
-    <row r="15" ht="24.95" customHeight="1" s="5">
+    <row r="15" ht="24.95" customHeight="1" s="7">
       <c r="A15" t="n">
         <v>1325933</v>
       </c>
@@ -1289,7 +1299,7 @@
         <v>42936</v>
       </c>
       <c r="I15" t="n">
-        <v>-515</v>
+        <v>-545</v>
       </c>
       <c r="J15">
         <f>IF(DAYS360(H15,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -1304,7 +1314,7 @@
         <v>44000.56388888889</v>
       </c>
     </row>
-    <row r="16" ht="24.95" customHeight="1" s="5">
+    <row r="16" ht="24.95" customHeight="1" s="7">
       <c r="A16" t="n">
         <v>1330487</v>
       </c>
@@ -1342,7 +1352,7 @@
         <v>42936</v>
       </c>
       <c r="I16" t="n">
-        <v>-515</v>
+        <v>-545</v>
       </c>
       <c r="J16">
         <f>IF(DAYS360(H16,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -1357,7 +1367,7 @@
         <v>44000.5625</v>
       </c>
     </row>
-    <row r="17" ht="24.95" customHeight="1" s="5">
+    <row r="17" ht="24.95" customHeight="1" s="7">
       <c r="A17" t="n">
         <v>1330047</v>
       </c>
@@ -1395,7 +1405,7 @@
         <v>42871</v>
       </c>
       <c r="I17" t="n">
-        <v>-580</v>
+        <v>-610</v>
       </c>
       <c r="J17">
         <f>IF(DAYS360(H17,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -1405,7 +1415,7 @@
         <v>43486.94791666666</v>
       </c>
     </row>
-    <row r="18" ht="24.95" customHeight="1" s="5">
+    <row r="18" ht="24.95" customHeight="1" s="7">
       <c r="A18" t="n">
         <v>1398517</v>
       </c>
@@ -1443,7 +1453,7 @@
         <v>40560</v>
       </c>
       <c r="I18" t="n">
-        <v>-2891</v>
+        <v>-2921</v>
       </c>
       <c r="J18">
         <f>IF(DAYS360(H18,TODAY(),FALSE)&gt;720,"VENCIDO","VIGENTE")</f>
@@ -1456,21 +1466,6 @@
       </c>
       <c r="L18" s="3" t="n">
         <v>41939.85</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="I24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="I25" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="I26" t="n">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1478,14 +1473,14 @@
     <mergeCell ref="A1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="J3:J18">
-    <cfRule type="cellIs" priority="4" operator="equal" dxfId="5">
-      <formula>"VIGENTE"</formula>
-    </cfRule>
     <cfRule type="expression" priority="1" dxfId="2">
       <formula>I3&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" priority="2" dxfId="3">
+    <cfRule type="expression" priority="2" dxfId="4">
       <formula>I3&lt;30</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3">
+      <formula>"VIGENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K18">
@@ -1525,37 +1520,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" style="5" min="1" max="1"/>
-    <col width="14" customWidth="1" style="5" min="2" max="2"/>
-    <col width="14.28515625" customWidth="1" style="5" min="3" max="3"/>
-    <col width="39.7109375" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
-    <col width="18.7109375" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col width="14.85546875" customWidth="1" style="5" min="6" max="6"/>
-    <col width="11.28515625" customWidth="1" style="5" min="7" max="7"/>
-    <col width="13" customWidth="1" style="5" min="8" max="8"/>
-    <col width="8.7109375" bestFit="1" customWidth="1" style="5" min="9" max="9"/>
-    <col width="10.42578125" customWidth="1" style="5" min="10" max="10"/>
-    <col width="12.5703125" customWidth="1" style="5" min="11" max="11"/>
-    <col width="21" customWidth="1" style="5" min="12" max="12"/>
-    <col width="12" customWidth="1" style="5" min="13" max="13"/>
+    <col width="10" customWidth="1" style="7" min="1" max="1"/>
+    <col width="14" customWidth="1" style="7" min="2" max="2"/>
+    <col width="14.28515625" customWidth="1" style="7" min="3" max="3"/>
+    <col width="39.7109375" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
+    <col width="18.7109375" bestFit="1" customWidth="1" style="7" min="5" max="5"/>
+    <col width="14.85546875" customWidth="1" style="7" min="6" max="6"/>
+    <col width="11.28515625" customWidth="1" style="7" min="7" max="7"/>
+    <col width="13" customWidth="1" style="7" min="8" max="8"/>
+    <col width="8.7109375" bestFit="1" customWidth="1" style="7" min="9" max="9"/>
+    <col width="10.42578125" customWidth="1" style="7" min="10" max="10"/>
+    <col width="12.5703125" customWidth="1" style="7" min="11" max="11"/>
+    <col width="21" customWidth="1" style="7" min="12" max="12"/>
+    <col width="12" customWidth="1" style="7" min="13" max="13"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.25" customHeight="1" s="5">
+    <row r="1" ht="23.25" customHeight="1" s="7">
       <c r="A1" s="6" t="inlineStr">
         <is>
           <t>RELACION DE SENSORES H2S (VIGENCIA 1 AÑO)</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="35.25" customHeight="1" s="5">
+    <row r="2" ht="35.25" customHeight="1" s="7">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Barcode</t>
@@ -1624,7 +1619,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="24.95" customHeight="1" s="5">
+    <row r="3" ht="24.95" customHeight="1" s="7">
       <c r="A3" t="n">
         <v>1334617</v>
       </c>
@@ -1662,7 +1657,7 @@
         <v>43843</v>
       </c>
       <c r="I3" t="n">
-        <v>27</v>
+        <v>-3</v>
       </c>
       <c r="J3">
         <f>IF(DAYS360(H3,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -1681,8 +1676,11 @@
           <t>****Se cambio fecha interna con fecha de calibracion el 22/03/20</t>
         </is>
       </c>
-    </row>
-    <row r="4" ht="24.95" customHeight="1" s="5">
+      <c r="R3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="24.95" customHeight="1" s="7">
       <c r="A4" t="n">
         <v>1327831</v>
       </c>
@@ -1720,7 +1718,7 @@
         <v>43843</v>
       </c>
       <c r="I4" t="n">
-        <v>27</v>
+        <v>-3</v>
       </c>
       <c r="J4">
         <f>IF(DAYS360(H4,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -1729,8 +1727,11 @@
       <c r="L4" s="3" t="n">
         <v>44060.6</v>
       </c>
-    </row>
-    <row r="5" ht="24.95" customHeight="1" s="5">
+      <c r="R4" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" ht="24.95" customHeight="1" s="7">
       <c r="A5" t="n">
         <v>1302688</v>
       </c>
@@ -1768,7 +1769,7 @@
         <v>43843</v>
       </c>
       <c r="I5" t="n">
-        <v>27</v>
+        <v>-3</v>
       </c>
       <c r="J5">
         <f>IF(DAYS360(H5,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -1777,8 +1778,11 @@
       <c r="L5" s="3" t="n">
         <v>43917.17916666667</v>
       </c>
-    </row>
-    <row r="6" ht="24.95" customHeight="1" s="5">
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="24.95" customHeight="1" s="7">
       <c r="A6" t="n">
         <v>1327935</v>
       </c>
@@ -1816,7 +1820,7 @@
         <v>43865</v>
       </c>
       <c r="I6" t="n">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="J6">
         <f>IF(DAYS360(H6,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -1826,7 +1830,7 @@
         <v>44060.6</v>
       </c>
     </row>
-    <row r="7" ht="24.95" customHeight="1" s="5">
+    <row r="7" ht="24.95" customHeight="1" s="7">
       <c r="A7" t="n">
         <v>1326418</v>
       </c>
@@ -1864,7 +1868,7 @@
         <v>41956</v>
       </c>
       <c r="I7" t="n">
-        <v>-1860</v>
+        <v>-1890</v>
       </c>
       <c r="J7">
         <f>IF(DAYS360(H7,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -1879,7 +1883,7 @@
         <v>44000.56388888889</v>
       </c>
     </row>
-    <row r="8" ht="24.95" customHeight="1" s="5">
+    <row r="8" ht="24.95" customHeight="1" s="7">
       <c r="A8" t="n">
         <v>1301239</v>
       </c>
@@ -1917,7 +1921,7 @@
         <v>42321</v>
       </c>
       <c r="I8" t="n">
-        <v>-1495</v>
+        <v>-1525</v>
       </c>
       <c r="J8">
         <f>IF(DAYS360(H8,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -1932,7 +1936,7 @@
         <v>44000.56319444445</v>
       </c>
     </row>
-    <row r="9" ht="24.95" customHeight="1" s="5">
+    <row r="9" ht="24.95" customHeight="1" s="7">
       <c r="A9" t="n">
         <v>1278988</v>
       </c>
@@ -1970,7 +1974,7 @@
         <v>42926</v>
       </c>
       <c r="I9" t="n">
-        <v>-890</v>
+        <v>-920</v>
       </c>
       <c r="J9">
         <f>IF(DAYS360(H9,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -1990,7 +1994,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="24.95" customHeight="1" s="5">
+    <row r="10" ht="24.95" customHeight="1" s="7">
       <c r="A10" t="n">
         <v>1329138</v>
       </c>
@@ -2028,7 +2032,7 @@
         <v>43111</v>
       </c>
       <c r="I10" t="n">
-        <v>-705</v>
+        <v>-735</v>
       </c>
       <c r="J10">
         <f>IF(DAYS360(H10,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2040,7 +2044,7 @@
         </is>
       </c>
       <c r="L10" s="3" t="n">
-        <v>44000.55833333333</v>
+        <v>44000.55833333332</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -2048,7 +2052,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="24.95" customHeight="1" s="5">
+    <row r="11" ht="24.95" customHeight="1" s="7">
       <c r="A11" t="n">
         <v>1317359</v>
       </c>
@@ -2086,7 +2090,7 @@
         <v>43500</v>
       </c>
       <c r="I11" t="n">
-        <v>-316</v>
+        <v>-346</v>
       </c>
       <c r="J11">
         <f>IF(DAYS360(H11,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2101,7 +2105,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="24.95" customHeight="1" s="5">
+    <row r="12" ht="24.95" customHeight="1" s="7">
       <c r="A12" t="n">
         <v>1313883</v>
       </c>
@@ -2139,7 +2143,7 @@
         <v>43500</v>
       </c>
       <c r="I12" t="n">
-        <v>-316</v>
+        <v>-346</v>
       </c>
       <c r="J12">
         <f>IF(DAYS360(H12,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2149,7 +2153,7 @@
         <v>44088.71111111111</v>
       </c>
     </row>
-    <row r="13" ht="24.95" customHeight="1" s="5">
+    <row r="13" ht="24.95" customHeight="1" s="7">
       <c r="A13" t="n">
         <v>1327896</v>
       </c>
@@ -2187,7 +2191,7 @@
         <v>43500</v>
       </c>
       <c r="I13" t="n">
-        <v>-316</v>
+        <v>-346</v>
       </c>
       <c r="J13">
         <f>IF(DAYS360(H13,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2197,7 +2201,7 @@
         <v>44088.71111111111</v>
       </c>
     </row>
-    <row r="14" ht="24.95" customHeight="1" s="5">
+    <row r="14" ht="24.95" customHeight="1" s="7">
       <c r="A14" t="n">
         <v>1457704</v>
       </c>
@@ -2235,7 +2239,7 @@
         <v>43529</v>
       </c>
       <c r="I14" t="n">
-        <v>-287</v>
+        <v>-317</v>
       </c>
       <c r="J14">
         <f>IF(DAYS360(H14,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2245,7 +2249,7 @@
         <v>43882.04166666666</v>
       </c>
     </row>
-    <row r="15" ht="24.95" customHeight="1" s="5">
+    <row r="15" ht="24.95" customHeight="1" s="7">
       <c r="A15" t="n">
         <v>1327708</v>
       </c>
@@ -2283,7 +2287,7 @@
         <v>43529</v>
       </c>
       <c r="I15" t="n">
-        <v>-287</v>
+        <v>-317</v>
       </c>
       <c r="J15">
         <f>IF(DAYS360(H15,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2293,7 +2297,7 @@
         <v>43882.04166666666</v>
       </c>
     </row>
-    <row r="16" ht="24.95" customHeight="1" s="5">
+    <row r="16" ht="24.95" customHeight="1" s="7">
       <c r="A16" t="n">
         <v>1302723</v>
       </c>
@@ -2326,7 +2330,7 @@
         <v>43539</v>
       </c>
       <c r="I16" t="n">
-        <v>-277</v>
+        <v>-307</v>
       </c>
       <c r="J16">
         <f>IF(DAYS360(H16,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2341,7 +2345,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="24.95" customHeight="1" s="5">
+    <row r="17" ht="24.95" customHeight="1" s="7">
       <c r="A17" t="n">
         <v>1329156</v>
       </c>
@@ -2379,7 +2383,7 @@
         <v>43607</v>
       </c>
       <c r="I17" t="n">
-        <v>-209</v>
+        <v>-239</v>
       </c>
       <c r="J17">
         <f>IF(DAYS360(H17,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2389,7 +2393,7 @@
         <v>43892.90902777778</v>
       </c>
     </row>
-    <row r="18" ht="24.95" customHeight="1" s="5">
+    <row r="18" ht="24.95" customHeight="1" s="7">
       <c r="A18" t="n">
         <v>1301390</v>
       </c>
@@ -2427,7 +2431,7 @@
         <v>43637</v>
       </c>
       <c r="I18" t="n">
-        <v>-179</v>
+        <v>-209</v>
       </c>
       <c r="J18">
         <f>IF(DAYS360(H18,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2437,7 +2441,7 @@
         <v>44088.71111111111</v>
       </c>
     </row>
-    <row r="19" ht="24.95" customHeight="1" s="5">
+    <row r="19" ht="24.95" customHeight="1" s="7">
       <c r="A19" t="n">
         <v>1327960</v>
       </c>
@@ -2475,7 +2479,7 @@
         <v>43666</v>
       </c>
       <c r="I19" t="n">
-        <v>-150</v>
+        <v>-180</v>
       </c>
       <c r="J19">
         <f>IF(DAYS360(H19,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2485,7 +2489,7 @@
         <v>44088.71041666667</v>
       </c>
     </row>
-    <row r="20" ht="24.95" customHeight="1" s="5">
+    <row r="20" ht="24.95" customHeight="1" s="7">
       <c r="A20" t="n">
         <v>1331438</v>
       </c>
@@ -2523,7 +2527,7 @@
         <v>43686</v>
       </c>
       <c r="I20" t="n">
-        <v>-130</v>
+        <v>-160</v>
       </c>
       <c r="J20">
         <f>IF(DAYS360(H20,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2533,7 +2537,7 @@
         <v>43882.04166666666</v>
       </c>
     </row>
-    <row r="21" ht="24.95" customHeight="1" s="5">
+    <row r="21" ht="24.95" customHeight="1" s="7">
       <c r="A21" t="n">
         <v>1316504</v>
       </c>
@@ -2571,7 +2575,7 @@
         <v>43791</v>
       </c>
       <c r="I21" t="n">
-        <v>-25</v>
+        <v>-55</v>
       </c>
       <c r="J21">
         <f>IF(DAYS360(H21,TODAY(),FALSE)&gt;360,"VENCIDO","VIGENTE")</f>
@@ -2579,21 +2583,6 @@
       </c>
       <c r="L21" s="3" t="n">
         <v>44126.89027777778</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="I24" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="I25" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="I26" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2601,14 +2590,14 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="J3:J21">
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="5">
-      <formula>"VIGENTE"</formula>
-    </cfRule>
     <cfRule type="expression" priority="1" dxfId="2">
       <formula>I3&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" priority="2" dxfId="3">
+    <cfRule type="expression" priority="2" dxfId="4">
       <formula>I3&lt;30</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="3">
+      <formula>"VIGENTE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K21">

</xml_diff>